<commit_message>
changed detail in excel
</commit_message>
<xml_diff>
--- a/Testes.xlsx
+++ b/Testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Red\Desktop\Investigacao2020\FeatureExtractionSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E154CE7-2A6F-4317-A015-152D92B97891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98A9A02-5203-42F3-993B-93A84860F190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C8C43D5-2640-471F-9E2F-B63DD0724C75}"/>
   </bookViews>
@@ -327,13 +327,13 @@
     <t>Vamos depois comparar cada bloco com o melhor e ver a media das diferenças da edit distance de cada frase</t>
   </si>
   <si>
-    <t>Se for menor que uma threshold (agora é 3) entao tiramos 10% ao bloco que tamos a comparar</t>
-  </si>
-  <si>
     <t>Se for maior, adicionamos 10% ao bloco que tamos a comparar e 10% ao bloco principal</t>
   </si>
   <si>
     <t>mc_ai.txt</t>
+  </si>
+  <si>
+    <t>Se for menor que uma threshold (sendo que a threshold é neste momento 30% da média do tamanho das frases do bloco principal) entao tiramos 10% ao bloco que tamos a comparar</t>
   </si>
 </sst>
 </file>
@@ -341,7 +341,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -427,7 +427,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -761,7 +761,7 @@
   <dimension ref="A1:W66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,7 +1526,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="12"/>
       <c r="F22" s="12"/>
@@ -1700,7 +1700,7 @@
       <c r="D31" s="6"/>
       <c r="E31"/>
       <c r="F31" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="D32" s="6"/>
       <c r="F32" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>

</xml_diff>